<commit_message>
v2.2: Professional chart enhancements with data labels, thicker lines, and optimized styling
</commit_message>
<xml_diff>
--- a/Portfolio report_Roth IRA_07.02.2026.xlsx
+++ b/Portfolio report_Roth IRA_07.02.2026.xlsx
@@ -227,7 +227,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -323,11 +323,55 @@
         <color rgb="00000000"/>
       </bottom>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
@@ -448,6 +492,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -581,6 +631,9 @@
               </a:ln>
             </spPr>
           </marker>
+          <dLbls>
+            <showVal val="1"/>
+          </dLbls>
           <cat>
             <strRef>
               <f>'Executive Summary'!$G$4:$G$15</f>
@@ -815,6 +868,9 @@
             </a:ln>
           </spPr>
           <invertIfNegative val="1"/>
+          <dLbls>
+            <showVal val="1"/>
+          </dLbls>
           <cat>
             <strRef>
               <f>'Executive Summary'!$J$4:$J$15</f>
@@ -1000,7 +1056,6 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="10"/>
   <chart>
     <title>
       <tx>
@@ -1122,7 +1177,6 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="10"/>
   <chart>
     <title>
       <tx>
@@ -1236,6 +1290,507 @@
 </chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Portfolio Growth - 12 Month Progression</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <lineChart>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Executive Summary'!H3</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="30000">
+              <a:solidFill>
+                <a:srgbClr val="1F4788"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Executive Summary'!$G$4:$G$15</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Executive Summary'!$H$4:$H$15</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </lineChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Month</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Portfolio Value ($)</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="b"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Monthly Returns - 12 Month Performance</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Executive Summary'!L3</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:srgbClr val="70AD47"/>
+            </a:solidFill>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Executive Summary'!$J$4:$J$15</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Executive Summary'!$L$4:$L$15</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <strRef>
+              <f>'Executive Summary'!M3</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:srgbClr val="C5504F"/>
+            </a:solidFill>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Executive Summary'!$J$4:$J$15</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Executive Summary'!$M$4:$M$15</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Month</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Profit ($)</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="b"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Portfolio Growth - 12 Month Progression</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <lineChart>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Executive Summary'!H3</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="30000">
+              <a:solidFill>
+                <a:srgbClr val="1F4788"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Executive Summary'!$G$4:$G$15</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Executive Summary'!$H$4:$H$15</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </lineChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Month</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Portfolio Value ($)</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="b"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Monthly Returns - 12 Month Performance</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Executive Summary'!K3</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:srgbClr val="4472C4"/>
+            </a:solidFill>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Executive Summary'!$J$4:$J$15</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Executive Summary'!$K$4:$K$15</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Month</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Profit ($)</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="b"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
@@ -1321,6 +1876,94 @@
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5760000" cy="3600000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="5" name="Chart 5"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>19</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5760000" cy="3600000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="6" name="Chart 6"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5760000" cy="3600000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="7" name="Chart 7"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>19</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5760000" cy="3600000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="8" name="Chart 8"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1618,7 +2261,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Q22" sqref="Q22"/>
@@ -1668,6 +2311,16 @@
           <t>Monthly Profit</t>
         </is>
       </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Gains</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Losses</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="22" customHeight="1" s="16">
       <c r="A4" s="28" t="inlineStr">
@@ -1691,6 +2344,12 @@
       <c r="K4" t="n">
         <v>-20980.1217</v>
       </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-20980.1217</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1" s="16">
       <c r="A5" s="29" t="inlineStr">
@@ -1724,6 +2383,12 @@
       <c r="K5" t="n">
         <v>6259.6203</v>
       </c>
+      <c r="L5" t="n">
+        <v>6259.6203</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" ht="18" customHeight="1" s="16">
       <c r="A6" s="30" t="inlineStr">
@@ -1757,6 +2422,12 @@
       <c r="K6" t="n">
         <v>17711.9694</v>
       </c>
+      <c r="L6" t="n">
+        <v>17711.9694</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" ht="18" customHeight="1" s="16">
       <c r="A7" s="30" t="inlineStr">
@@ -1790,6 +2461,12 @@
       <c r="K7" t="n">
         <v>15461.9381</v>
       </c>
+      <c r="L7" t="n">
+        <v>15461.9381</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" ht="18" customHeight="1" s="16">
       <c r="A8" s="30" t="inlineStr">
@@ -1823,6 +2500,12 @@
       <c r="K8" t="n">
         <v>12076.79056</v>
       </c>
+      <c r="L8" t="n">
+        <v>12076.79056</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" ht="18" customHeight="1" s="16">
       <c r="A9" s="30" t="inlineStr">
@@ -1856,6 +2539,12 @@
       <c r="K9" t="n">
         <v>4094.15154</v>
       </c>
+      <c r="L9" t="n">
+        <v>4094.15154</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" ht="18" customHeight="1" s="16">
       <c r="A10" s="30" t="inlineStr">
@@ -1889,6 +2578,12 @@
       <c r="K10" t="n">
         <v>10459.462681</v>
       </c>
+      <c r="L10" t="n">
+        <v>10459.462681</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" ht="18" customHeight="1" s="16">
       <c r="A11" s="30" t="inlineStr">
@@ -1922,6 +2617,12 @@
       <c r="K11" t="n">
         <v>5264.7273334</v>
       </c>
+      <c r="L11" t="n">
+        <v>5264.7273334</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" ht="18" customHeight="1" s="16">
       <c r="A12" s="30" t="inlineStr">
@@ -1955,6 +2656,12 @@
       <c r="K12" t="n">
         <v>-570.87454</v>
       </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>-570.87454</v>
+      </c>
     </row>
     <row r="13" ht="18" customHeight="1" s="16">
       <c r="A13" s="30" t="inlineStr">
@@ -1988,6 +2695,12 @@
       <c r="K13" t="n">
         <v>-2553.8761341</v>
       </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>-2553.8761341</v>
+      </c>
     </row>
     <row r="14" ht="18" customHeight="1" s="16">
       <c r="A14" s="30" t="inlineStr">
@@ -2021,6 +2734,12 @@
       <c r="K14" t="n">
         <v>8804.315811300001</v>
       </c>
+      <c r="L14" t="n">
+        <v>8804.315811300001</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" ht="8" customHeight="1" s="16">
       <c r="G15" t="inlineStr">
@@ -2038,6 +2757,12 @@
       </c>
       <c r="K15" t="n">
         <v>2830.70742500182</v>
+      </c>
+      <c r="L15" t="n">
+        <v>2830.70742500182</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16" ht="21.95" customHeight="1" s="16">
@@ -2104,8 +2829,8 @@
         </is>
       </c>
     </row>
-    <row r="23" ht="20" customHeight="1" s="16">
-      <c r="A23" s="33" t="inlineStr">
+    <row r="23" ht="32" customHeight="1" s="16">
+      <c r="A23" s="45" t="inlineStr">
         <is>
           <t>1. Portfolio demonstrates consistent positive growth with strong cumulative returns</t>
         </is>
@@ -2115,8 +2840,8 @@
       <c r="D23" s="34" t="n"/>
       <c r="E23" s="34" t="n"/>
     </row>
-    <row r="24" ht="20" customHeight="1" s="16">
-      <c r="A24" s="33" t="inlineStr">
+    <row r="24" ht="32" customHeight="1" s="16">
+      <c r="A24" s="45" t="inlineStr">
         <is>
           <t>2. High win rate (83%+ positive months) indicates favorable market positioning</t>
         </is>
@@ -2126,8 +2851,8 @@
       <c r="D24" s="34" t="n"/>
       <c r="E24" s="34" t="n"/>
     </row>
-    <row r="25" ht="20" customHeight="1" s="16">
-      <c r="A25" s="33" t="inlineStr">
+    <row r="25" ht="32" customHeight="1" s="16">
+      <c r="A25" s="45" t="inlineStr">
         <is>
           <t>3. Dividend accumulation provides steady passive income stream</t>
         </is>
@@ -2137,8 +2862,8 @@
       <c r="D25" s="34" t="n"/>
       <c r="E25" s="34" t="n"/>
     </row>
-    <row r="26" ht="20" customHeight="1" s="16">
-      <c r="A26" s="33" t="inlineStr">
+    <row r="26" ht="32" customHeight="1" s="16">
+      <c r="A26" s="45" t="inlineStr">
         <is>
           <t>4. Average monthly returns exceed typical market benchmarks</t>
         </is>
@@ -2148,8 +2873,8 @@
       <c r="D26" s="34" t="n"/>
       <c r="E26" s="34" t="n"/>
     </row>
-    <row r="27" ht="20" customHeight="1" s="16">
-      <c r="A27" s="33" t="inlineStr">
+    <row r="27" ht="32" customHeight="1" s="16">
+      <c r="A27" s="45" t="inlineStr">
         <is>
           <t>5. Trading activity shows disciplined approach with measured transactions</t>
         </is>
@@ -2159,8 +2884,8 @@
       <c r="D27" s="34" t="n"/>
       <c r="E27" s="34" t="n"/>
     </row>
-    <row r="28" ht="20" customHeight="1" s="16">
-      <c r="A28" s="33" t="inlineStr">
+    <row r="28" ht="32" customHeight="1" s="16">
+      <c r="A28" s="45" t="inlineStr">
         <is>
           <t>6. Risk management evident from contained worst-month losses relative to gains</t>
         </is>
@@ -2178,8 +2903,8 @@
         </is>
       </c>
     </row>
-    <row r="31" ht="20" customHeight="1" s="16">
-      <c r="A31" s="35" t="inlineStr">
+    <row r="31" ht="32" customHeight="1" s="16">
+      <c r="A31" s="46" t="inlineStr">
         <is>
           <t>1. Continue current strategy - proven track record of consistent returns</t>
         </is>
@@ -2189,8 +2914,8 @@
       <c r="D31" s="36" t="n"/>
       <c r="E31" s="36" t="n"/>
     </row>
-    <row r="32" ht="20" customHeight="1" s="16">
-      <c r="A32" s="35" t="inlineStr">
+    <row r="32" ht="32" customHeight="1" s="16">
+      <c r="A32" s="46" t="inlineStr">
         <is>
           <t>2. Maintain dividend reinvestment for compound growth acceleration</t>
         </is>
@@ -2200,8 +2925,8 @@
       <c r="D32" s="36" t="n"/>
       <c r="E32" s="36" t="n"/>
     </row>
-    <row r="33" ht="20" customHeight="1" s="16">
-      <c r="A33" s="35" t="inlineStr">
+    <row r="33" ht="32" customHeight="1" s="16">
+      <c r="A33" s="46" t="inlineStr">
         <is>
           <t>3. Review quarterly performance against benchmarks (S&amp;P 500, Russell 2000)</t>
         </is>
@@ -2211,8 +2936,8 @@
       <c r="D33" s="36" t="n"/>
       <c r="E33" s="36" t="n"/>
     </row>
-    <row r="34" ht="20" customHeight="1" s="16">
-      <c r="A34" s="35" t="inlineStr">
+    <row r="34" ht="32" customHeight="1" s="16">
+      <c r="A34" s="46" t="inlineStr">
         <is>
           <t>4. Rebalance portfolio if allocation drifts &gt;10% from target</t>
         </is>
@@ -2222,8 +2947,8 @@
       <c r="D34" s="36" t="n"/>
       <c r="E34" s="36" t="n"/>
     </row>
-    <row r="35" ht="20" customHeight="1" s="16">
-      <c r="A35" s="35" t="inlineStr">
+    <row r="35" ht="32" customHeight="1" s="16">
+      <c r="A35" s="46" t="inlineStr">
         <is>
           <t>5. Evaluate tax-loss harvesting opportunities in down months</t>
         </is>
@@ -2233,8 +2958,8 @@
       <c r="D35" s="36" t="n"/>
       <c r="E35" s="36" t="n"/>
     </row>
-    <row r="36" ht="20" customHeight="1" s="16">
-      <c r="A36" s="35" t="inlineStr">
+    <row r="36" ht="32" customHeight="1" s="16">
+      <c r="A36" s="46" t="inlineStr">
         <is>
           <t>6. Monitor market conditions for tactical adjustments if warranted</t>
         </is>

</xml_diff>